<commit_message>
Nat upate in follow-up
</commit_message>
<xml_diff>
--- a/Output/section1.xlsx
+++ b/Output/section1.xlsx
@@ -3,25 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\2. Data-work\R-workspace\WITM\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE53BDB6-4667-4BA7-85A4-4DEFD8FF3849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36E603F-DA92-44EB-9608-9D3BE21A473A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1380" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1380" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="q1" sheetId="1" r:id="rId1"/>
-    <sheet name="q4" r:id="rId5" sheetId="2"/>
+    <sheet name="q4" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="76">
   <si>
     <t>Consent</t>
   </si>
@@ -135,14 +135,127 @@
   </si>
   <si>
     <t>Anti-caste</t>
+  </si>
+  <si>
+    <t>Ignoro estas categorias que obtienen el 90% de las respestas y no discriminan</t>
+  </si>
+  <si>
+    <t>General HR subjects</t>
+  </si>
+  <si>
+    <t>Feminist specifit subjects</t>
+  </si>
+  <si>
+    <t>Intersectionality (minority groups)</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.anti_caste</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.anti_militarization</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.black_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.climate_justice</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.crisis_response</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.countering_anti_gender</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.digital_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.disability_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.displaced_migrant_refugee_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.economic_justice</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.information_media_freedom</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.harm_reduction</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.end_gender_violence</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.pleasure_bodily_care</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.resisting_war_on_drugs</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.rights_for_people_living_with_hiv</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.holistic_safety_protection_collective_care</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.human_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.indigenous_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.intersex_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.labour_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.lesbian_bisexual_queer_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.racial_justice</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.religious_ethnic_minority_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.sex_workers_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.srhr_bodily_autonomy</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.trans_non_binary_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.womens_rights</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.young_feminists</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.girls_movements</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.hr_defenders_at_risk</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing.98</t>
+  </si>
+  <si>
+    <t>q4_forms_organizing_spc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sexual and reproductive health &amp; rights (and othershealth rights) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -150,13 +263,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -186,9 +327,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,7 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
@@ -570,14 +718,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="60.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" customWidth="1"/>
+    <col min="13" max="13" width="55.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -587,360 +743,803 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="n">
-        <v>314.0</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2" s="3">
+        <v>314</v>
+      </c>
+      <c r="C2" s="3">
         <v>78.3</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>114</v>
+      </c>
+      <c r="I2">
+        <v>28.4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="n">
-        <v>275.0</v>
-      </c>
-      <c r="C3" t="n">
-        <v>68.6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="B3" s="3">
+        <v>275</v>
+      </c>
+      <c r="C3" s="3">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>152</v>
+      </c>
+      <c r="I3">
+        <v>37.9</v>
+      </c>
+      <c r="J3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="n">
-        <v>238.0</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4" s="3">
+        <v>238</v>
+      </c>
+      <c r="C4" s="3">
         <v>59.4</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>91</v>
+      </c>
+      <c r="I4">
+        <v>22.7</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="n">
-        <v>223.0</v>
-      </c>
-      <c r="C5" t="n">
+      <c r="B5" s="5">
+        <v>223</v>
+      </c>
+      <c r="C5" s="5">
         <v>55.6</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+      <c r="G5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="5">
+        <v>103</v>
+      </c>
+      <c r="I5" s="5">
+        <v>25.7</v>
+      </c>
+      <c r="J5" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="n">
-        <v>152.0</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="B6" s="5">
+        <v>152</v>
+      </c>
+      <c r="C6" s="5">
         <v>37.9</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
+      <c r="G6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="5">
+        <v>97</v>
+      </c>
+      <c r="I6" s="5">
+        <v>24.2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>66</v>
+      </c>
+      <c r="M6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="n">
-        <v>145.0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>36.2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
+      <c r="B7" s="5">
+        <v>145</v>
+      </c>
+      <c r="C7" s="5">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7">
+        <v>75</v>
+      </c>
+      <c r="I7">
+        <v>18.7</v>
+      </c>
+      <c r="J7" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="n">
-        <v>136.0</v>
-      </c>
-      <c r="C8" t="n">
+      <c r="B8" s="5">
+        <v>136</v>
+      </c>
+      <c r="C8" s="5">
         <v>33.9</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
+      <c r="G8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="5">
+        <v>46</v>
+      </c>
+      <c r="I8" s="5">
+        <v>11.5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="n">
-        <v>131.0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>32.7</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
+      <c r="B9" s="5">
+        <v>131</v>
+      </c>
+      <c r="C9" s="5">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="n">
-        <v>114.0</v>
-      </c>
-      <c r="C10" t="n">
+      <c r="B10" s="5">
+        <v>114</v>
+      </c>
+      <c r="C10" s="5">
         <v>28.4</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10">
+        <v>145</v>
+      </c>
+      <c r="I10">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="J10" t="s">
+        <v>72</v>
+      </c>
+      <c r="M10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="n">
-        <v>112.0</v>
-      </c>
-      <c r="C11" t="n">
+      <c r="B11" s="5">
+        <v>112</v>
+      </c>
+      <c r="C11" s="5">
         <v>27.9</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11">
+        <v>136</v>
+      </c>
+      <c r="I11">
+        <v>33.9</v>
+      </c>
+      <c r="J11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="n">
-        <v>103.0</v>
-      </c>
-      <c r="C12" t="n">
+      <c r="B12" s="5">
+        <v>103</v>
+      </c>
+      <c r="C12" s="5">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12">
+        <v>131</v>
+      </c>
+      <c r="I12">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="J12" t="s">
+        <v>45</v>
+      </c>
+      <c r="M12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="n">
-        <v>97.0</v>
-      </c>
-      <c r="C13" t="n">
+      <c r="B13" s="5">
+        <v>97</v>
+      </c>
+      <c r="C13" s="5">
         <v>24.2</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13">
+        <v>44</v>
+      </c>
+      <c r="I13">
+        <v>11</v>
+      </c>
+      <c r="J13" t="s">
+        <v>43</v>
+      </c>
+      <c r="M13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="n">
-        <v>91.0</v>
-      </c>
-      <c r="C14" t="n">
+      <c r="B14" s="5">
+        <v>91</v>
+      </c>
+      <c r="C14" s="5">
         <v>22.7</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14">
+        <v>78</v>
+      </c>
+      <c r="I14">
+        <v>19.5</v>
+      </c>
+      <c r="J14" t="s">
+        <v>46</v>
+      </c>
+      <c r="M14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="n">
-        <v>87.0</v>
-      </c>
-      <c r="C15" t="n">
+      <c r="B15" s="5">
+        <v>87</v>
+      </c>
+      <c r="C15" s="5">
         <v>21.7</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
+      <c r="G15" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15">
+        <v>19</v>
+      </c>
+      <c r="I15">
+        <v>4.7</v>
+      </c>
+      <c r="J15" t="s">
+        <v>56</v>
+      </c>
+      <c r="M15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="n">
-        <v>85.0</v>
-      </c>
-      <c r="C16" t="n">
+      <c r="B16" s="5">
+        <v>85</v>
+      </c>
+      <c r="C16" s="5">
         <v>21.2</v>
       </c>
-    </row>
-    <row r="17">
+      <c r="G16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="I16">
+        <v>3.5</v>
+      </c>
+      <c r="J16" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="n">
-        <v>84.0</v>
-      </c>
-      <c r="C17" t="n">
+      <c r="B17">
+        <v>84</v>
+      </c>
+      <c r="C17">
         <v>20.9</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17">
+        <v>72</v>
+      </c>
+      <c r="I17">
+        <v>18</v>
+      </c>
+      <c r="J17" t="s">
+        <v>48</v>
+      </c>
+      <c r="M17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="C18" t="n">
+      <c r="B18" s="5">
+        <v>78</v>
+      </c>
+      <c r="C18" s="5">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
+      <c r="G18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H18">
+        <v>59</v>
+      </c>
+      <c r="I18">
+        <v>14.7</v>
+      </c>
+      <c r="J18" t="s">
+        <v>52</v>
+      </c>
+      <c r="M18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B19" t="n">
-        <v>75.0</v>
-      </c>
-      <c r="C19" t="n">
+      <c r="B19" s="5">
+        <v>75</v>
+      </c>
+      <c r="C19" s="5">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
+      <c r="M19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B20" t="n">
-        <v>75.0</v>
-      </c>
-      <c r="C20" t="n">
+      <c r="B20" s="5">
+        <v>75</v>
+      </c>
+      <c r="C20" s="5">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
+      <c r="G20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="n">
-        <v>73.0</v>
-      </c>
-      <c r="C21" t="n">
+      <c r="B21" s="5">
+        <v>73</v>
+      </c>
+      <c r="C21" s="5">
         <v>18.2</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
+      <c r="G21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21">
+        <v>112</v>
+      </c>
+      <c r="I21">
+        <v>27.9</v>
+      </c>
+      <c r="J21" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="n">
-        <v>72.0</v>
-      </c>
-      <c r="C22" t="n">
-        <v>18.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
+      <c r="B22" s="5">
+        <v>72</v>
+      </c>
+      <c r="C22" s="5">
+        <v>18</v>
+      </c>
+      <c r="G22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22">
+        <v>87</v>
+      </c>
+      <c r="I22">
+        <v>21.7</v>
+      </c>
+      <c r="J22" t="s">
+        <v>50</v>
+      </c>
+      <c r="M22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B23" t="n">
-        <v>59.0</v>
-      </c>
-      <c r="C23" t="n">
+      <c r="B23" s="5">
+        <v>59</v>
+      </c>
+      <c r="C23" s="5">
         <v>14.7</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23">
+        <v>85</v>
+      </c>
+      <c r="I23">
+        <v>21.2</v>
+      </c>
+      <c r="J23" t="s">
+        <v>60</v>
+      </c>
+      <c r="M23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B24" t="n">
-        <v>56.0</v>
-      </c>
-      <c r="C24" t="n">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
+      <c r="B24" s="5">
+        <v>56</v>
+      </c>
+      <c r="C24" s="5">
+        <v>14</v>
+      </c>
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24">
+        <v>56</v>
+      </c>
+      <c r="I24">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>64</v>
+      </c>
+      <c r="M24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B25" t="n">
-        <v>54.0</v>
-      </c>
-      <c r="C25" t="n">
+      <c r="B25" s="5">
+        <v>54</v>
+      </c>
+      <c r="C25" s="5">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="26">
+      <c r="G25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25">
+        <v>54</v>
+      </c>
+      <c r="I25">
+        <v>13.5</v>
+      </c>
+      <c r="J25" t="s">
+        <v>44</v>
+      </c>
+      <c r="M25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="n">
-        <v>50.0</v>
-      </c>
-      <c r="C26" t="n">
+      <c r="B26">
+        <v>50</v>
+      </c>
+      <c r="C26">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="27">
+      <c r="G26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26">
+        <v>35</v>
+      </c>
+      <c r="I26">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J26" t="s">
+        <v>65</v>
+      </c>
+      <c r="M26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B27" t="n">
-        <v>48.0</v>
-      </c>
-      <c r="C27" t="n">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
+      <c r="B27">
+        <v>48</v>
+      </c>
+      <c r="C27">
+        <v>12</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B28" t="n">
-        <v>46.0</v>
-      </c>
-      <c r="C28" t="n">
+      <c r="B28" s="5">
+        <v>46</v>
+      </c>
+      <c r="C28" s="5">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="29">
+      <c r="G28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28">
+        <v>84</v>
+      </c>
+      <c r="I28">
+        <v>20.9</v>
+      </c>
+      <c r="J28" t="s">
+        <v>57</v>
+      </c>
+      <c r="M28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>33</v>
       </c>
-      <c r="B29" t="n">
-        <v>44.0</v>
-      </c>
-      <c r="C29" t="n">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="30">
+      <c r="B29">
+        <v>44</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="G29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29">
+        <v>73</v>
+      </c>
+      <c r="I29">
+        <v>18.2</v>
+      </c>
+      <c r="J29" t="s">
+        <v>58</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>34</v>
       </c>
-      <c r="B30" t="n">
-        <v>35.0</v>
-      </c>
-      <c r="C30" t="n">
-        <v>8.7</v>
-      </c>
-    </row>
-    <row r="31">
+      <c r="B30">
+        <v>35</v>
+      </c>
+      <c r="C30">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="G30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30">
+        <v>48</v>
+      </c>
+      <c r="I30">
+        <v>12</v>
+      </c>
+      <c r="J30" t="s">
+        <v>55</v>
+      </c>
+      <c r="M30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31">
+        <v>19</v>
+      </c>
+      <c r="C31">
+        <v>4.7</v>
+      </c>
+      <c r="G31" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>223</v>
+      </c>
+      <c r="I31">
+        <v>55.6</v>
+      </c>
+      <c r="J31" t="s">
+        <v>67</v>
+      </c>
+      <c r="M31" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>3.5</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="M32" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>35</v>
       </c>
-      <c r="B31" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="C31" t="n">
+      <c r="B33">
+        <v>22</v>
+      </c>
+      <c r="C33">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="C32" t="n">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" t="n">
-        <v>14.0</v>
-      </c>
-      <c r="C33" t="n">
-        <v>3.5</v>
+      <c r="M33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M34" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
+    <sortCondition descending="1" ref="C2:C32"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="D2:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>